<commit_message>
Fix Yield data for Temora simulations
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/GxExM/GrainWt.xlsx
+++ b/Tests/Validation/Wheat/GxExM/GrainWt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/hut104_csiro_au/Documents/Work/GRDC WheatYieldPhysiology/Simulations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\Validation\Wheat\GxExM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:1_{91926DCE-977E-4E5B-A859-BF79AAEB6891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E343E62A-200A-4FEB-99D9-B2ABF890FFD8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C678DD0-2ACB-4211-B1F1-514139F8567E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$AB$121</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I661"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38:H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1934,20 +1934,20 @@
         <v>13</v>
       </c>
       <c r="E38">
-        <v>398</v>
+        <v>335.75</v>
       </c>
       <c r="F38">
-        <v>31.759513010540111</v>
+        <v>38.248093634410942</v>
       </c>
       <c r="G38">
-        <v>2.1500000000000002E-2</v>
+        <v>2.1499999999999998E-2</v>
       </c>
       <c r="H38">
-        <v>1.9148542155126335E-3</v>
+        <v>1.9148542155126762E-3</v>
       </c>
       <c r="I38">
         <f t="shared" si="0"/>
-        <v>18511.627906976744</v>
+        <v>15616.279069767443</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
@@ -1964,20 +1964,20 @@
         <v>14</v>
       </c>
       <c r="E39">
-        <v>370.5</v>
+        <v>303.75</v>
       </c>
       <c r="F39">
-        <v>70.793125843309582</v>
+        <v>58.180036667800977</v>
       </c>
       <c r="G39">
-        <v>2.1249999999999998E-2</v>
+        <v>2.1250000000000002E-2</v>
       </c>
       <c r="H39">
-        <v>2.9860788111948362E-3</v>
+        <v>2.9860788111948193E-3</v>
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>17435.294117647059</v>
+        <v>14294.117647058822</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
@@ -1994,20 +1994,20 @@
         <v>12</v>
       </c>
       <c r="E40">
-        <v>389.5</v>
+        <v>316</v>
       </c>
       <c r="F40">
-        <v>23.014488190413157</v>
+        <v>27.141603981096377</v>
       </c>
       <c r="G40">
-        <v>2.1500000000000002E-2</v>
+        <v>2.1499999999999998E-2</v>
       </c>
       <c r="H40">
-        <v>9.9999999999992174E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>18116.279069767439</v>
+        <v>14697.674418604653</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
@@ -2024,20 +2024,20 @@
         <v>10</v>
       </c>
       <c r="E41">
-        <v>555.75</v>
+        <v>481.5</v>
       </c>
       <c r="F41">
-        <v>103.01253968975493</v>
+        <v>36.299678602801251</v>
       </c>
       <c r="G41">
         <v>2.8750000000000001E-2</v>
       </c>
       <c r="H41">
-        <v>4.27200187265877E-3</v>
+        <v>4.2720018726587648E-3</v>
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
-        <v>19330.434782608696</v>
+        <v>16747.82608695652</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
@@ -2054,20 +2054,20 @@
         <v>8</v>
       </c>
       <c r="E42">
-        <v>430.25</v>
+        <v>422</v>
       </c>
       <c r="F42">
-        <v>46.94944089123959</v>
+        <v>44.624358071946908</v>
       </c>
       <c r="G42">
         <v>2.775E-2</v>
       </c>
       <c r="H42">
-        <v>9.574271077563639E-4</v>
+        <v>9.5742710775633809E-4</v>
       </c>
       <c r="I42">
         <f t="shared" si="0"/>
-        <v>15504.504504504504</v>
+        <v>15207.207207207208</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
@@ -2084,20 +2084,20 @@
         <v>4</v>
       </c>
       <c r="E43">
-        <v>517.75</v>
+        <v>420.25</v>
       </c>
       <c r="F43">
-        <v>33.836617246212228</v>
+        <v>23.171462333367451</v>
       </c>
       <c r="G43">
         <v>3.075E-2</v>
       </c>
       <c r="H43">
-        <v>1.4999999999999792E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="I43">
         <f t="shared" si="0"/>
-        <v>16837.398373983739</v>
+        <v>13666.666666666666</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
@@ -2114,20 +2114,20 @@
         <v>7</v>
       </c>
       <c r="E44">
-        <v>327.25</v>
+        <v>293.75</v>
       </c>
       <c r="F44">
-        <v>28.300471138598851</v>
+        <v>59.106542221088638</v>
       </c>
       <c r="G44">
         <v>2.1749999999999999E-2</v>
       </c>
       <c r="H44">
-        <v>2.0615528128088445E-3</v>
+        <v>2.0615528128088301E-3</v>
       </c>
       <c r="I44">
         <f t="shared" si="0"/>
-        <v>15045.977011494253</v>
+        <v>13505.747126436783</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
@@ -2144,20 +2144,20 @@
         <v>2</v>
       </c>
       <c r="E45">
-        <v>505.5</v>
+        <v>460</v>
       </c>
       <c r="F45">
-        <v>37.995613781944186</v>
+        <v>31.379398762032817</v>
       </c>
       <c r="G45">
         <v>2.725E-2</v>
       </c>
       <c r="H45">
-        <v>1.7078251276599829E-3</v>
+        <v>1.707825127659933E-3</v>
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
-        <v>18550.458715596331</v>
+        <v>16880.733944954129</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
@@ -2174,20 +2174,20 @@
         <v>3</v>
       </c>
       <c r="E46">
-        <v>449.5</v>
+        <v>399.75</v>
       </c>
       <c r="F46">
-        <v>26.006409466386039</v>
+        <v>40.90130397269342</v>
       </c>
       <c r="G46">
         <v>2.4E-2</v>
       </c>
       <c r="H46">
-        <v>1.9999999999999879E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="I46">
         <f t="shared" si="0"/>
-        <v>18729.166666666668</v>
+        <v>16656.25</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
@@ -2204,20 +2204,20 @@
         <v>5</v>
       </c>
       <c r="E47">
-        <v>453.5</v>
+        <v>399.75</v>
       </c>
       <c r="F47">
-        <v>31.22498999199199</v>
+        <v>38.055879966176057</v>
       </c>
       <c r="G47">
         <v>2.9749999999999999E-2</v>
       </c>
       <c r="H47">
-        <v>3.7749172176354054E-3</v>
+        <v>3.774917217635375E-3</v>
       </c>
       <c r="I47">
         <f t="shared" si="0"/>
-        <v>15243.697478991597</v>
+        <v>13436.974789915967</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
@@ -2234,20 +2234,20 @@
         <v>9</v>
       </c>
       <c r="E48">
-        <v>326.75</v>
+        <v>310.33333333333331</v>
       </c>
       <c r="F48">
-        <v>49.701609631882143</v>
+        <v>58.226568964119316</v>
       </c>
       <c r="G48">
-        <v>2.1750000000000002E-2</v>
+        <v>2.1749999999999999E-2</v>
       </c>
       <c r="H48">
-        <v>2.753785273643037E-3</v>
+        <v>2.7537852736430508E-3</v>
       </c>
       <c r="I48">
         <f t="shared" si="0"/>
-        <v>15022.988505747126</v>
+        <v>14268.199233716476</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
@@ -2264,20 +2264,20 @@
         <v>6</v>
       </c>
       <c r="E49">
-        <v>390</v>
+        <v>303.25</v>
       </c>
       <c r="F49">
-        <v>62.785348609369052</v>
+        <v>58.829556063824469</v>
       </c>
       <c r="G49">
         <v>2.325E-2</v>
       </c>
       <c r="H49">
-        <v>3.2015621187164224E-3</v>
+        <v>3.2015621187164241E-3</v>
       </c>
       <c r="I49">
         <f t="shared" si="0"/>
-        <v>16774.193548387098</v>
+        <v>13043.010752688173</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
@@ -5868,5 +5868,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;KFF0000 UNOFFICIAL&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Aptos"&amp;12&amp;KFF0000 UNOFFICIAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>